<commit_message>
feat: add manual test cases for testing UI with different usernames
</commit_message>
<xml_diff>
--- a/Testdata/TestData.xlsx
+++ b/Testdata/TestData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>qcu24s4901FyWDTwXGr6XA==</t>
-  </si>
-  <si>
-    <t>locked_out_user</t>
   </si>
   <si>
     <t>problem_user</t>
@@ -54,7 +51,6 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -75,9 +71,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -292,13 +286,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="20.13"/>
     <col customWidth="1" min="2" max="2" width="25.88"/>
+    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -306,7 +301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -314,7 +309,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -322,7 +317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -330,7 +325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -338,19 +333,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>